<commit_message>
Added a script as an alternative for parsing
</commit_message>
<xml_diff>
--- a/master_functions/getAccountListRequest.xlsx
+++ b/master_functions/getAccountListRequest.xlsx
@@ -1,33 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="29005"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kafagy/Documents/work/eVAS-Automation/master_functions/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="16600" yWindow="2200" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Version</t>
   </si>
@@ -40,18 +27,12 @@
   <si>
     <t>Client</t>
   </si>
-  <si>
-    <t>GSI</t>
-  </si>
-  <si>
-    <t>Glory</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,11 +69,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -139,12 +115,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -171,15 +147,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -206,7 +181,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,16 +356,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,20 +377,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1.3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>